<commit_message>
Initial checkin of new formDef executor. Updates to many supporting libraries.
</commit_message>
<xml_diff>
--- a/form-files/breathcounter/breathcounter.xlsx
+++ b/form-files/breathcounter/breathcounter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="480" windowWidth="11196" windowHeight="5244" activeTab="2"/>
+    <workbookView xWindow="2592" yWindow="624" windowWidth="11196" windowHeight="5244" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>type</t>
   </si>
@@ -24,12 +24,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>hint</t>
-  </si>
-  <si>
     <t>breathcounter</t>
   </si>
   <si>
@@ -42,15 +36,9 @@
     <t>Custom prompt behavior is specified in the customPromptTypes.js file and we require a model to be defined on the prompt_types sheet.</t>
   </si>
   <si>
-    <t>schema.type</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
-    <t>setting</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -60,10 +48,25 @@
     <t>form_version</t>
   </si>
   <si>
-    <t>form_title</t>
-  </si>
-  <si>
     <t>Breathcounter</t>
+  </si>
+  <si>
+    <t>setting_name</t>
+  </si>
+  <si>
+    <t>display.title</t>
+  </si>
+  <si>
+    <t>survey</t>
+  </si>
+  <si>
+    <t>prompt_type_name</t>
+  </si>
+  <si>
+    <t>display.text</t>
+  </si>
+  <si>
+    <t>display.hint</t>
   </si>
 </sst>
 </file>
@@ -102,11 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,9 +414,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="27.109375" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
@@ -420,32 +426,32 @@
     <col min="4" max="4" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -455,32 +461,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="21.44140625" customWidth="1"/>
     <col min="2" max="2" width="49.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -488,49 +498,55 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
+    <row r="1" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    <row r="4" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>